<commit_message>
added inc time to test file and changed dir for test file
</commit_message>
<xml_diff>
--- a/xml-automation/automatic_xml_creator/Template_Juergen_Sandy_test.xlsx
+++ b/xml-automation/automatic_xml_creator/Template_Juergen_Sandy_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\melc-automation\xml-automation\automatic_xml_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A8A4B6-A10F-4E9D-B580-F76907A69ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E029B7A-DE4F-45D5-9111-1434F6CA9DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -973,49 +973,49 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,25 +1566,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="46" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
     </row>
     <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -1632,7 +1632,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34">
+      <c r="A3" s="38">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1641,18 +1641,18 @@
       <c r="C3" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="35" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="12">
         <v>10</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="41">
         <f>60-G5</f>
         <v>60</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="34">
+      <c r="H3" s="38">
         <v>900</v>
       </c>
       <c r="I3" s="16">
@@ -1666,20 +1666,20 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="12">
         <v>10</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="43"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="16">
         <v>600</v>
       </c>
@@ -1691,20 +1691,20 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="47"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="12">
         <v>10</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="43"/>
+      <c r="H5" s="39"/>
       <c r="I5" s="10">
         <v>0</v>
       </c>
@@ -1716,20 +1716,20 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="45"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="12">
         <v>10</v>
       </c>
-      <c r="F6" s="42"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="44"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="10">
         <v>0</v>
       </c>
@@ -1786,7 +1786,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
+      <c r="A8" s="38">
         <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -1795,13 +1795,13 @@
       <c r="C8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="35" t="s">
         <v>69</v>
       </c>
       <c r="E8" s="12">
         <v>50</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="41">
         <f>60-G8-G9-G10-G11</f>
         <v>43.2</v>
       </c>
@@ -1809,7 +1809,7 @@
         <f>2*(60/E8)</f>
         <v>2.4</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="38">
         <v>3300</v>
       </c>
       <c r="I8" s="16">
@@ -1833,23 +1833,23 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="11" t="s">
         <v>57</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="47"/>
       <c r="E9" s="12">
         <v>50</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="13">
         <f>2*(60/E9)</f>
         <v>2.4</v>
       </c>
-      <c r="H9" s="43"/>
+      <c r="H9" s="39"/>
       <c r="I9" s="16">
         <v>300</v>
       </c>
@@ -1871,23 +1871,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="38"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="12">
         <v>10</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="13">
         <f>2*(60/E10)</f>
         <v>12</v>
       </c>
-      <c r="H10" s="43"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="10">
         <v>300</v>
       </c>
@@ -1905,22 +1905,22 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="48"/>
       <c r="E11" s="12">
         <v>10000</v>
       </c>
-      <c r="F11" s="42"/>
+      <c r="F11" s="43"/>
       <c r="G11" s="13">
         <v>0</v>
       </c>
-      <c r="H11" s="44"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="16">
         <v>1</v>
       </c>
@@ -1932,7 +1932,7 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34">
+      <c r="A12" s="38">
         <v>4</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1941,13 +1941,13 @@
       <c r="C12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="35" t="s">
         <v>82</v>
       </c>
       <c r="E12" s="12">
         <v>50</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="41">
         <f>60-G12-G13-G14</f>
         <v>54.900000000000006</v>
       </c>
@@ -1955,7 +1955,7 @@
         <f t="shared" ref="G12:G29" si="2">2*(60/E12)</f>
         <v>2.4</v>
       </c>
-      <c r="H12" s="34">
+      <c r="H12" s="38">
         <v>3300</v>
       </c>
       <c r="I12" s="16">
@@ -1977,23 +1977,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="38"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="12">
         <v>400</v>
       </c>
-      <c r="F13" s="41"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="13">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="H13" s="43"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="10">
         <v>600</v>
       </c>
@@ -2015,23 +2015,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="39"/>
+      <c r="D14" s="48"/>
       <c r="E14" s="12">
         <v>50</v>
       </c>
-      <c r="F14" s="42"/>
+      <c r="F14" s="43"/>
       <c r="G14" s="13">
         <f t="shared" si="2"/>
         <v>2.4</v>
       </c>
-      <c r="H14" s="44"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="16">
         <v>300</v>
       </c>
@@ -2098,7 +2098,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34">
+      <c r="A16" s="38">
         <v>6</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -2107,13 +2107,13 @@
       <c r="C16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="35" t="s">
         <v>96</v>
       </c>
       <c r="E16" s="12">
         <v>100</v>
       </c>
-      <c r="F16" s="40">
+      <c r="F16" s="41">
         <f>60-G16-G17</f>
         <v>56.4</v>
       </c>
@@ -2121,7 +2121,7 @@
         <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="H16" s="34">
+      <c r="H16" s="38">
         <v>3300</v>
       </c>
       <c r="I16" s="10">
@@ -2143,23 +2143,23 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="45"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="12">
         <v>50</v>
       </c>
-      <c r="F17" s="44"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="13">
         <f t="shared" si="2"/>
         <v>2.4</v>
       </c>
-      <c r="H17" s="44"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="10">
         <v>600</v>
       </c>
@@ -2179,7 +2179,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34">
+      <c r="A18" s="38">
         <v>7</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -2188,13 +2188,13 @@
       <c r="C18" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="35" t="s">
         <v>104</v>
       </c>
       <c r="E18" s="12">
         <v>100</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="41">
         <f>60-G18-G19</f>
         <v>58.199999999999996</v>
       </c>
@@ -2202,7 +2202,7 @@
         <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="H18" s="34">
+      <c r="H18" s="38">
         <v>3300</v>
       </c>
       <c r="I18" s="16">
@@ -2224,23 +2224,23 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="45"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="12">
         <v>200</v>
       </c>
-      <c r="F19" s="44"/>
+      <c r="F19" s="40"/>
       <c r="G19" s="13">
         <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="H19" s="44"/>
+      <c r="H19" s="40"/>
       <c r="I19" s="10">
         <v>600</v>
       </c>
@@ -2258,7 +2258,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34">
+      <c r="A20" s="38">
         <v>8</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -2267,13 +2267,13 @@
       <c r="C20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="35" t="s">
         <v>108</v>
       </c>
       <c r="E20" s="12">
         <v>200</v>
       </c>
-      <c r="F20" s="40">
+      <c r="F20" s="41">
         <f>60-G20-G21</f>
         <v>58.199999999999996</v>
       </c>
@@ -2281,7 +2281,7 @@
         <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="38">
         <v>3300</v>
       </c>
       <c r="I20" s="16">
@@ -2303,23 +2303,23 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
+      <c r="A21" s="45"/>
       <c r="B21" s="17" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="45"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="12">
         <v>100</v>
       </c>
-      <c r="F21" s="44"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="13">
         <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="H21" s="44"/>
+      <c r="H21" s="40"/>
       <c r="I21" s="10">
         <v>900</v>
       </c>
@@ -2863,7 +2863,9 @@
         <f t="shared" ref="G33" si="7">2*(60/E33)</f>
         <v>0.6</v>
       </c>
-      <c r="H33" s="10"/>
+      <c r="H33" s="10">
+        <v>3000</v>
+      </c>
       <c r="I33" s="16">
         <v>600</v>
       </c>
@@ -2977,7 +2979,7 @@
       </c>
     </row>
     <row r="36" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34">
+      <c r="A36" s="38">
         <v>23</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -2986,13 +2988,13 @@
       <c r="C36" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="37" t="s">
+      <c r="D36" s="35" t="s">
         <v>153</v>
       </c>
       <c r="E36" s="12">
         <v>50</v>
       </c>
-      <c r="F36" s="40">
+      <c r="F36" s="41">
         <f>60-G36-G37</f>
         <v>57</v>
       </c>
@@ -3000,7 +3002,7 @@
         <f t="shared" si="6"/>
         <v>2.4</v>
       </c>
-      <c r="H36" s="34">
+      <c r="H36" s="38">
         <v>3000</v>
       </c>
       <c r="I36" s="10">
@@ -3020,23 +3022,23 @@
       </c>
     </row>
     <row r="37" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="45"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="12">
         <v>200</v>
       </c>
-      <c r="F37" s="42"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="13">
         <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
-      <c r="H37" s="44"/>
+      <c r="H37" s="40"/>
       <c r="I37" s="16">
         <v>600</v>
       </c>
@@ -3154,7 +3156,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="34">
+      <c r="A40" s="38">
         <v>26</v>
       </c>
       <c r="B40" s="11" t="s">
@@ -3163,13 +3165,13 @@
       <c r="C40" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="37" t="s">
+      <c r="D40" s="35" t="s">
         <v>157</v>
       </c>
       <c r="E40" s="12">
         <v>200</v>
       </c>
-      <c r="F40" s="40">
+      <c r="F40" s="41">
         <f>60-G40-G41-G42</f>
         <v>57.9</v>
       </c>
@@ -3177,7 +3179,7 @@
         <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
-      <c r="H40" s="34">
+      <c r="H40" s="38">
         <v>1800</v>
       </c>
       <c r="I40" s="16">
@@ -3199,23 +3201,23 @@
       </c>
     </row>
     <row r="41" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="47"/>
+      <c r="D41" s="36"/>
       <c r="E41" s="12">
         <v>100</v>
       </c>
-      <c r="F41" s="41"/>
+      <c r="F41" s="42"/>
       <c r="G41" s="13">
         <f t="shared" si="6"/>
         <v>1.2</v>
       </c>
-      <c r="H41" s="43"/>
+      <c r="H41" s="39"/>
       <c r="I41" s="10">
         <v>300</v>
       </c>
@@ -3237,23 +3239,23 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
+      <c r="A42" s="45"/>
       <c r="B42" s="11" t="s">
         <v>199</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="D42" s="45"/>
+      <c r="D42" s="37"/>
       <c r="E42" s="12">
         <v>400</v>
       </c>
-      <c r="F42" s="42"/>
+      <c r="F42" s="43"/>
       <c r="G42" s="13">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="H42" s="44"/>
+      <c r="H42" s="40"/>
       <c r="I42" s="10">
         <v>300</v>
       </c>
@@ -3278,7 +3280,7 @@
       <c r="G43" s="22"/>
       <c r="H43" s="23">
         <f>SUM(H5:H42)*1.1</f>
-        <v>71280</v>
+        <v>74580</v>
       </c>
       <c r="I43" s="24">
         <f>SUM(I5:I42)</f>
@@ -3301,7 +3303,7 @@
       <c r="G44" s="22"/>
       <c r="H44" s="23">
         <f>H43/60</f>
-        <v>1188</v>
+        <v>1243</v>
       </c>
       <c r="I44" s="23">
         <f>I43/60</f>
@@ -3324,7 +3326,7 @@
       <c r="G45" s="22"/>
       <c r="H45" s="23">
         <f>H44/60</f>
-        <v>19.8</v>
+        <v>20.716666666666665</v>
       </c>
       <c r="I45" s="23" t="e">
         <f>(I44/60)*#REF!</f>
@@ -3403,6 +3405,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="H36:H37"/>
     <mergeCell ref="J1:O1"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="H3:H6"/>
@@ -3419,24 +3439,6 @@
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="F20:F21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="H8:H11"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A1:I1 C3:C1048576">

</xml_diff>